<commit_message>
How to extract all caps names from a string.
</commit_message>
<xml_diff>
--- a/ExtractAllCapsNames.xlsx
+++ b/ExtractAllCapsNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C1B9E9-B614-4096-8634-592EFD29748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CA5E57-18CB-48E0-AE8E-72BF0DDAB192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -18,11 +18,12 @@
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="fxCap">_xlfn.LAMBDA(_xlpm.str,         _xlfn.LET(              _xlpm.x, _xlfn.TEXTSPLIT(_xlpm.str,," "),              _xlpm.y, _xlfn.MAP(_xlpm.x,_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.z,MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x),1,1),1),--AND((ROWS(_xlpm.z)&gt;1)*(CODE(_xlpm.z)&gt;=65)*(CODE(_xlpm.z)&lt;=90))))),              _xlfn.TEXTJOIN(" ",TRUE,_xlfn._xlws.FILTER(_xlpm.x,_xlpm.y=1))         )        )</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -782,7 +783,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1074,10 +1075,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1086,7 @@
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1096,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1106,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1115,7 +1116,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1124,14 +1125,10 @@
         <v>December 18 - Destroyer PARTRIDGE (1,540t, 22/2/42), sunk by U-boat torpedo, W Mediterranean</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D11" t="str" cm="1">
         <f t="array" ref="D11:D23">_xlfn.TEXTSPLIT(C8,," ")</f>
         <v>December</v>
-      </c>
-      <c r="E11" t="b" cm="1">
-        <f t="array" ref="E11:E23">EXACT(_xlfn.ANCHORARRAY(D11),UPPER(_xlfn.ANCHORARRAY(D11)))</f>
-        <v>0</v>
       </c>
       <c r="F11" cm="1">
         <f t="array" ref="F11:F23">_xlfn.MAP(_xlfn.ANCHORARRAY(D11),_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.z,MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x),1,1),1),
@@ -1143,17 +1140,32 @@
         <f t="array" ref="H11">_xlfn.TEXTJOIN(" ",TRUE,_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(D11),_xlfn.ANCHORARRAY(F11)=1))</f>
         <v>PARTRIDGE</v>
       </c>
-      <c r="K11" t="str">
-        <f>H11</f>
+      <c r="K11" t="str" cm="1">
+        <f t="array" ref="K11">fxCap(C8)</f>
         <v>PARTRIDGE</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N11" t="str" cm="1">
+        <f t="array" ref="N11">_xlfn.LAMBDA(_xlpm.str,
+        _xlfn.LET(
+             _xlpm.x, _xlfn.TEXTSPLIT(_xlpm.str,," "),
+             _xlpm.y, _xlfn.MAP(_xlpm.x,_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.z,MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x),1,1),1),--AND((ROWS(_xlpm.z)&gt;1)*(CODE(_xlpm.z)&gt;=65)*(CODE(_xlpm.z)&lt;=90))))),
+             _xlfn.TEXTJOIN(" ",TRUE,_xlfn._xlws.FILTER(_xlpm.x,_xlpm.y=1))
+        )
+       )(C8)</f>
+        <v>PARTRIDGE</v>
+      </c>
+      <c r="P11" t="str" cm="1">
+        <f t="array" ref="P11">fxCap(C8)</f>
+        <v>PARTRIDGE</v>
+      </c>
+      <c r="R11" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(P11)</f>
+        <v>=fxCap(C8)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D12" t="str">
         <v>18</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1166,13 +1178,10 @@
         <v>LCM</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D13" t="str">
         <v>-</v>
       </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
       <c r="F13">
         <v>0</v>
       </c>
@@ -1183,13 +1192,10 @@
         <v>MARIGOLD</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D14" t="str">
         <v>Destroyer</v>
       </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
       <c r="F14">
         <v>0</v>
       </c>
@@ -1200,13 +1206,10 @@
         <v>BLEAN</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <v>PARTRIDGE</v>
       </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
       <c r="F15">
         <v>1</v>
       </c>
@@ -1217,12 +1220,9 @@
         <v>TRAVELLER</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <v>(1,540t,</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1238,9 +1238,6 @@
       <c r="D17" t="str">
         <v>22/2/42),</v>
       </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
       <c r="F17">
         <v>0</v>
       </c>
@@ -1255,9 +1252,6 @@
       <c r="D18" t="str">
         <v>sunk</v>
       </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
       <c r="F18">
         <v>0</v>
       </c>
@@ -1266,9 +1260,6 @@
       <c r="D19" t="str">
         <v>by</v>
       </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
       <c r="F19">
         <v>0</v>
       </c>
@@ -1277,9 +1268,6 @@
       <c r="D20" t="str">
         <v>U-boat</v>
       </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
       <c r="F20">
         <v>0</v>
       </c>
@@ -1288,9 +1276,6 @@
       <c r="D21" t="str">
         <v>torpedo,</v>
       </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
       <c r="F21">
         <v>0</v>
       </c>
@@ -1299,9 +1284,6 @@
       <c r="D22" t="str">
         <v>W</v>
       </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
       <c r="F22">
         <v>0</v>
       </c>
@@ -1309,9 +1291,6 @@
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
         <v>Mediterranean</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>

</xml_diff>

<commit_message>
This was useful as a technique for extracting numbers from text
</commit_message>
<xml_diff>
--- a/ExtractAllCapsNames.xlsx
+++ b/ExtractAllCapsNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CA5E57-18CB-48E0-AE8E-72BF0DDAB192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FE19E-4F64-4963-8290-FFA1275A01BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -157,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -240,18 +240,6 @@
       <name val="Consolas"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -347,7 +335,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -357,8 +345,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -783,7 +769,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1077,8 +1063,8 @@
   </sheetPr>
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1096,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>45311</v>
       </c>
       <c r="C3" s="2"/>
@@ -1300,7 +1286,7 @@
       <c r="A38">
         <v>1</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1316,7 +1302,7 @@
       <c r="A40">
         <v>3</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1336,11 +1322,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>